<commit_message>
Drop any rows where the SID is nan.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="248">
   <si>
     <t>company_name</t>
   </si>
@@ -1115,7 +1115,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F145"/>
+  <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3998,14 +3998,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="3:5">
-      <c r="C145" t="s">
-        <v>230</v>
-      </c>
-      <c r="E145">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rewrote sessions() function to take pandas columns as arguments instead of using pandas apply().  This seems to be faster, still need to rewrite pages_per_session().
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="247">
   <si>
     <t>company_name</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Sessions</t>
-  </si>
-  <si>
-    <t>Pages / Session</t>
   </si>
   <si>
     <t>Signature Consultants</t>
@@ -1115,13 +1112,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F144"/>
+  <dimension ref="A1:E144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1137,19 +1134,16 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D2">
         <v>1874506</v>
@@ -1157,19 +1151,16 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D3">
         <v>88581275</v>
@@ -1177,19 +1168,16 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D4">
         <v>2277</v>
@@ -1197,19 +1185,16 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D5">
         <v>94943308</v>
@@ -1217,19 +1202,16 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D6">
         <v>9643371</v>
@@ -1237,19 +1219,16 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D7">
         <v>3487433</v>
@@ -1257,19 +1236,16 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D8">
         <v>29015547</v>
@@ -1277,19 +1253,16 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D9">
         <v>10710256</v>
@@ -1297,19 +1270,16 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D10">
         <v>22837572</v>
@@ -1317,19 +1287,16 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D11">
         <v>120220674</v>
@@ -1337,19 +1304,16 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D12">
         <v>87584491</v>
@@ -1357,19 +1321,16 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D13">
         <v>62481418</v>
@@ -1377,19 +1338,16 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D14">
         <v>18304937</v>
@@ -1397,19 +1355,16 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D15">
         <v>76260666</v>
@@ -1417,19 +1372,16 @@
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D16">
         <v>122882133</v>
@@ -1437,19 +1389,16 @@
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D17">
         <v>427654</v>
@@ -1457,19 +1406,16 @@
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D18">
         <v>1274211</v>
@@ -1477,19 +1423,16 @@
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D19">
         <v>63243298</v>
@@ -1497,19 +1440,16 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D20">
         <v>107353422</v>
@@ -1517,19 +1457,16 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D21">
         <v>114279008</v>
@@ -1537,19 +1474,16 @@
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D22">
         <v>62276135</v>
@@ -1557,19 +1491,16 @@
       <c r="E22">
         <v>1</v>
       </c>
-      <c r="F22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D23">
         <v>61131136</v>
@@ -1577,19 +1508,16 @@
       <c r="E23">
         <v>1</v>
       </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D24">
         <v>8334706</v>
@@ -1597,19 +1525,16 @@
       <c r="E24">
         <v>1</v>
       </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D25">
         <v>120294900</v>
@@ -1617,16 +1542,13 @@
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D26">
         <v>123181958</v>
@@ -1634,19 +1556,16 @@
       <c r="E26">
         <v>1</v>
       </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D27">
         <v>59014</v>
@@ -1654,19 +1573,16 @@
       <c r="E27">
         <v>1</v>
       </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D28">
         <v>118357638</v>
@@ -1674,19 +1590,16 @@
       <c r="E28">
         <v>1</v>
       </c>
-      <c r="F28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D29">
         <v>50919072</v>
@@ -1694,19 +1607,16 @@
       <c r="E29">
         <v>1</v>
       </c>
-      <c r="F29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D30">
         <v>206865</v>
@@ -1714,19 +1624,16 @@
       <c r="E30">
         <v>1</v>
       </c>
-      <c r="F30">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D31">
         <v>55091</v>
@@ -1734,19 +1641,16 @@
       <c r="E31">
         <v>1</v>
       </c>
-      <c r="F31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D32">
         <v>23077089</v>
@@ -1754,19 +1658,16 @@
       <c r="E32">
         <v>1</v>
       </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D33">
         <v>324782</v>
@@ -1774,19 +1675,16 @@
       <c r="E33">
         <v>1</v>
       </c>
-      <c r="F33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D34">
         <v>50792754</v>
@@ -1794,19 +1692,16 @@
       <c r="E34">
         <v>1</v>
       </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D35">
         <v>1657209</v>
@@ -1814,19 +1709,16 @@
       <c r="E35">
         <v>1</v>
       </c>
-      <c r="F35">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C36" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D36">
         <v>29363767</v>
@@ -1834,19 +1726,16 @@
       <c r="E36">
         <v>1</v>
       </c>
-      <c r="F36">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D37">
         <v>119753147</v>
@@ -1854,19 +1743,16 @@
       <c r="E37">
         <v>1</v>
       </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D38">
         <v>8813570</v>
@@ -1874,19 +1760,16 @@
       <c r="E38">
         <v>1</v>
       </c>
-      <c r="F38">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C39" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D39">
         <v>9716409</v>
@@ -1894,19 +1777,16 @@
       <c r="E39">
         <v>1</v>
       </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C40" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D40">
         <v>3439734</v>
@@ -1914,19 +1794,16 @@
       <c r="E40">
         <v>1</v>
       </c>
-      <c r="F40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C41" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D41">
         <v>28166261</v>
@@ -1934,19 +1811,16 @@
       <c r="E41">
         <v>1</v>
       </c>
-      <c r="F41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D42">
         <v>110164086</v>
@@ -1954,19 +1828,16 @@
       <c r="E42">
         <v>1</v>
       </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D43">
         <v>65549391</v>
@@ -1974,19 +1845,16 @@
       <c r="E43">
         <v>1</v>
       </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C44" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D44">
         <v>152167</v>
@@ -1994,19 +1862,16 @@
       <c r="E44">
         <v>1</v>
       </c>
-      <c r="F44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D45">
         <v>3546637</v>
@@ -2014,19 +1879,16 @@
       <c r="E45">
         <v>1</v>
       </c>
-      <c r="F45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D46">
         <v>672468</v>
@@ -2034,19 +1896,16 @@
       <c r="E46">
         <v>1</v>
       </c>
-      <c r="F46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C47" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D47">
         <v>88581346</v>
@@ -2054,19 +1913,16 @@
       <c r="E47">
         <v>1</v>
       </c>
-      <c r="F47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C48" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D48">
         <v>333292</v>
@@ -2074,19 +1930,16 @@
       <c r="E48">
         <v>1</v>
       </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C49" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D49">
         <v>120353825</v>
@@ -2094,19 +1947,16 @@
       <c r="E49">
         <v>1</v>
       </c>
-      <c r="F49">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C50" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D50">
         <v>114803999</v>
@@ -2114,19 +1964,16 @@
       <c r="E50">
         <v>1</v>
       </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C51" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D51">
         <v>121066621</v>
@@ -2134,19 +1981,16 @@
       <c r="E51">
         <v>1</v>
       </c>
-      <c r="F51">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C52" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D52">
         <v>114363338</v>
@@ -2154,19 +1998,16 @@
       <c r="E52">
         <v>1</v>
       </c>
-      <c r="F52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D53">
         <v>8870506</v>
@@ -2174,19 +2015,16 @@
       <c r="E53">
         <v>1</v>
       </c>
-      <c r="F53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C54" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D54">
         <v>9636101</v>
@@ -2194,19 +2032,16 @@
       <c r="E54">
         <v>1</v>
       </c>
-      <c r="F54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C55" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D55">
         <v>24505728</v>
@@ -2214,19 +2049,16 @@
       <c r="E55">
         <v>1</v>
       </c>
-      <c r="F55">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C56" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D56">
         <v>114413047</v>
@@ -2234,19 +2066,16 @@
       <c r="E56">
         <v>1</v>
       </c>
-      <c r="F56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C57" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D57">
         <v>3383279</v>
@@ -2254,19 +2083,16 @@
       <c r="E57">
         <v>1</v>
       </c>
-      <c r="F57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D58">
         <v>18261037</v>
@@ -2274,19 +2100,16 @@
       <c r="E58">
         <v>1</v>
       </c>
-      <c r="F58">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B59" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C59" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D59">
         <v>50792693</v>
@@ -2294,19 +2117,16 @@
       <c r="E59">
         <v>1</v>
       </c>
-      <c r="F59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C60" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D60">
         <v>65419794</v>
@@ -2314,19 +2134,16 @@
       <c r="E60">
         <v>1</v>
       </c>
-      <c r="F60">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C61" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D61">
         <v>111937346</v>
@@ -2334,19 +2151,16 @@
       <c r="E61">
         <v>1</v>
       </c>
-      <c r="F61">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C62" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D62">
         <v>25049946</v>
@@ -2354,19 +2168,16 @@
       <c r="E62">
         <v>1</v>
       </c>
-      <c r="F62">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C63" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D63">
         <v>62142906</v>
@@ -2374,19 +2185,16 @@
       <c r="E63">
         <v>1</v>
       </c>
-      <c r="F63">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C64" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D64">
         <v>411470</v>
@@ -2394,19 +2202,16 @@
       <c r="E64">
         <v>1</v>
       </c>
-      <c r="F64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C65" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D65">
         <v>77504470</v>
@@ -2414,19 +2219,16 @@
       <c r="E65">
         <v>1</v>
       </c>
-      <c r="F65">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C66" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D66">
         <v>110129535</v>
@@ -2434,19 +2236,16 @@
       <c r="E66">
         <v>1</v>
       </c>
-      <c r="F66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C67" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D67">
         <v>61358666</v>
@@ -2454,19 +2253,16 @@
       <c r="E67">
         <v>1</v>
       </c>
-      <c r="F67">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C68" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D68">
         <v>116578742</v>
@@ -2474,19 +2270,16 @@
       <c r="E68">
         <v>1</v>
       </c>
-      <c r="F68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C69" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D69">
         <v>62085175</v>
@@ -2494,19 +2287,16 @@
       <c r="E69">
         <v>1</v>
       </c>
-      <c r="F69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D70">
         <v>75933854</v>
@@ -2514,19 +2304,16 @@
       <c r="E70">
         <v>1</v>
       </c>
-      <c r="F70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D71">
         <v>75925683</v>
@@ -2534,19 +2321,16 @@
       <c r="E71">
         <v>1</v>
       </c>
-      <c r="F71">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C72" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D72">
         <v>62192622</v>
@@ -2554,19 +2338,16 @@
       <c r="E72">
         <v>1</v>
       </c>
-      <c r="F72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C73" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D73">
         <v>3474028</v>
@@ -2574,19 +2355,16 @@
       <c r="E73">
         <v>1</v>
       </c>
-      <c r="F73">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C74" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D74">
         <v>2120924</v>
@@ -2594,19 +2372,16 @@
       <c r="E74">
         <v>1</v>
       </c>
-      <c r="F74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C75" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D75">
         <v>574762</v>
@@ -2614,19 +2389,16 @@
       <c r="E75">
         <v>1</v>
       </c>
-      <c r="F75">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C76" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D76">
         <v>119309550</v>
@@ -2634,19 +2406,16 @@
       <c r="E76">
         <v>1</v>
       </c>
-      <c r="F76">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C77" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D77">
         <v>79984352</v>
@@ -2654,19 +2423,16 @@
       <c r="E77">
         <v>1</v>
       </c>
-      <c r="F77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C78" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D78">
         <v>96316606</v>
@@ -2674,19 +2440,16 @@
       <c r="E78">
         <v>1</v>
       </c>
-      <c r="F78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C79" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D79">
         <v>121239002</v>
@@ -2694,19 +2457,16 @@
       <c r="E79">
         <v>1</v>
       </c>
-      <c r="F79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C80" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D80">
         <v>65690454</v>
@@ -2714,19 +2474,16 @@
       <c r="E80">
         <v>1</v>
       </c>
-      <c r="F80">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C81" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D81">
         <v>48861</v>
@@ -2734,19 +2491,16 @@
       <c r="E81">
         <v>1</v>
       </c>
-      <c r="F81">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C82" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D82">
         <v>441104</v>
@@ -2754,19 +2508,16 @@
       <c r="E82">
         <v>1</v>
       </c>
-      <c r="F82">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C83" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D83">
         <v>417598</v>
@@ -2774,19 +2525,16 @@
       <c r="E83">
         <v>1</v>
       </c>
-      <c r="F83">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C84" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D84">
         <v>282236</v>
@@ -2794,19 +2542,16 @@
       <c r="E84">
         <v>1</v>
       </c>
-      <c r="F84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B85" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C85" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D85">
         <v>3617</v>
@@ -2814,19 +2559,16 @@
       <c r="E85">
         <v>1</v>
       </c>
-      <c r="F85">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C86" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D86">
         <v>64789992</v>
@@ -2834,19 +2576,16 @@
       <c r="E86">
         <v>1</v>
       </c>
-      <c r="F86">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C87" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D87">
         <v>53478381</v>
@@ -2854,19 +2593,16 @@
       <c r="E87">
         <v>1</v>
       </c>
-      <c r="F87">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C88" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D88">
         <v>74750637</v>
@@ -2874,19 +2610,16 @@
       <c r="E88">
         <v>1</v>
       </c>
-      <c r="F88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C89" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D89">
         <v>24551256</v>
@@ -2894,19 +2627,16 @@
       <c r="E89">
         <v>1</v>
       </c>
-      <c r="F89">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C90" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D90">
         <v>27515672</v>
@@ -2914,19 +2644,16 @@
       <c r="E90">
         <v>1</v>
       </c>
-      <c r="F90">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C91" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D91">
         <v>285202</v>
@@ -2934,19 +2661,16 @@
       <c r="E91">
         <v>1</v>
       </c>
-      <c r="F91">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C92" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D92">
         <v>330734</v>
@@ -2954,19 +2678,16 @@
       <c r="E92">
         <v>1</v>
       </c>
-      <c r="F92">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C93" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D93">
         <v>66899178</v>
@@ -2974,19 +2695,16 @@
       <c r="E93">
         <v>1</v>
       </c>
-      <c r="F93">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C94" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D94">
         <v>23781648</v>
@@ -2994,19 +2712,16 @@
       <c r="E94">
         <v>1</v>
       </c>
-      <c r="F94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C95" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D95">
         <v>89580408</v>
@@ -3014,19 +2729,16 @@
       <c r="E95">
         <v>1</v>
       </c>
-      <c r="F95">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C96" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D96">
         <v>59702148</v>
@@ -3034,19 +2746,16 @@
       <c r="E96">
         <v>1</v>
       </c>
-      <c r="F96">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C97" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D97">
         <v>29344533</v>
@@ -3054,19 +2763,16 @@
       <c r="E97">
         <v>1</v>
       </c>
-      <c r="F97">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C98" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D98">
         <v>3652496</v>
@@ -3074,19 +2780,16 @@
       <c r="E98">
         <v>1</v>
       </c>
-      <c r="F98">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B99" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C99" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D99">
         <v>115048979</v>
@@ -3094,19 +2797,16 @@
       <c r="E99">
         <v>1</v>
       </c>
-      <c r="F99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B100" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C100" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D100">
         <v>122253967</v>
@@ -3114,19 +2814,16 @@
       <c r="E100">
         <v>1</v>
       </c>
-      <c r="F100">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C101" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D101">
         <v>76317857</v>
@@ -3134,19 +2831,16 @@
       <c r="E101">
         <v>1</v>
       </c>
-      <c r="F101">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B102" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C102" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D102">
         <v>28916725</v>
@@ -3154,19 +2848,16 @@
       <c r="E102">
         <v>1</v>
       </c>
-      <c r="F102">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6">
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C103" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D103">
         <v>116500972</v>
@@ -3174,19 +2865,16 @@
       <c r="E103">
         <v>1</v>
       </c>
-      <c r="F103">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B104" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C104" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D104">
         <v>121155406</v>
@@ -3194,19 +2882,16 @@
       <c r="E104">
         <v>1</v>
       </c>
-      <c r="F104">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C105" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D105">
         <v>113083468</v>
@@ -3214,19 +2899,16 @@
       <c r="E105">
         <v>1</v>
       </c>
-      <c r="F105">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B106" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C106" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D106">
         <v>121500828</v>
@@ -3234,19 +2916,16 @@
       <c r="E106">
         <v>1</v>
       </c>
-      <c r="F106">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B107" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C107" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D107">
         <v>61673614</v>
@@ -3254,19 +2933,16 @@
       <c r="E107">
         <v>1</v>
       </c>
-      <c r="F107">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B108" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C108" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D108">
         <v>107353754</v>
@@ -3274,19 +2950,16 @@
       <c r="E108">
         <v>1</v>
       </c>
-      <c r="F108">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B109" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C109" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D109">
         <v>94430121</v>
@@ -3294,19 +2967,16 @@
       <c r="E109">
         <v>1</v>
       </c>
-      <c r="F109">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6">
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C110" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D110">
         <v>30166573</v>
@@ -3314,19 +2984,16 @@
       <c r="E110">
         <v>1</v>
       </c>
-      <c r="F110">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B111" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C111" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D111">
         <v>1874075</v>
@@ -3334,19 +3001,16 @@
       <c r="E111">
         <v>1</v>
       </c>
-      <c r="F111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B112" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C112" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D112">
         <v>63056166</v>
@@ -3354,19 +3018,16 @@
       <c r="E112">
         <v>1</v>
       </c>
-      <c r="F112">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C113" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D113">
         <v>73509114</v>
@@ -3374,19 +3035,16 @@
       <c r="E113">
         <v>1</v>
       </c>
-      <c r="F113">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B114" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C114" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D114">
         <v>4009456</v>
@@ -3394,19 +3052,16 @@
       <c r="E114">
         <v>1</v>
       </c>
-      <c r="F114">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B115" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C115" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D115">
         <v>63237387</v>
@@ -3414,19 +3069,16 @@
       <c r="E115">
         <v>1</v>
       </c>
-      <c r="F115">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B116" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C116" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D116">
         <v>61659652</v>
@@ -3434,19 +3086,16 @@
       <c r="E116">
         <v>1</v>
       </c>
-      <c r="F116">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B117" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C117" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D117">
         <v>121092023</v>
@@ -3454,19 +3103,16 @@
       <c r="E117">
         <v>1</v>
       </c>
-      <c r="F117">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B118" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C118" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D118">
         <v>10615945</v>
@@ -3474,19 +3120,16 @@
       <c r="E118">
         <v>1</v>
       </c>
-      <c r="F118">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B119" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C119" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D119">
         <v>60358057</v>
@@ -3494,19 +3137,16 @@
       <c r="E119">
         <v>1</v>
       </c>
-      <c r="F119">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B120" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C120" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D120">
         <v>114799829</v>
@@ -3514,19 +3154,16 @@
       <c r="E120">
         <v>1</v>
       </c>
-      <c r="F120">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
+    </row>
+    <row r="121" spans="1:5">
       <c r="A121" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B121" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C121" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D121">
         <v>3840295</v>
@@ -3534,19 +3171,16 @@
       <c r="E121">
         <v>1</v>
       </c>
-      <c r="F121">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B122" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C122" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D122">
         <v>29684833</v>
@@ -3554,19 +3188,16 @@
       <c r="E122">
         <v>1</v>
       </c>
-      <c r="F122">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
+    </row>
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B123" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C123" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D123">
         <v>22983616</v>
@@ -3574,19 +3205,16 @@
       <c r="E123">
         <v>1</v>
       </c>
-      <c r="F123">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
+    </row>
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B124" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C124" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D124">
         <v>10020982</v>
@@ -3594,19 +3222,16 @@
       <c r="E124">
         <v>1</v>
       </c>
-      <c r="F124">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
+    </row>
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B125" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C125" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D125">
         <v>121070994</v>
@@ -3614,19 +3239,16 @@
       <c r="E125">
         <v>1</v>
       </c>
-      <c r="F125">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B126" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C126" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D126">
         <v>1047511</v>
@@ -3634,19 +3256,16 @@
       <c r="E126">
         <v>2</v>
       </c>
-      <c r="F126">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B127" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C127" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D127">
         <v>78172883</v>
@@ -3654,19 +3273,16 @@
       <c r="E127">
         <v>2</v>
       </c>
-      <c r="F127">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6">
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B128" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C128" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D128">
         <v>37515</v>
@@ -3674,19 +3290,16 @@
       <c r="E128">
         <v>1</v>
       </c>
-      <c r="F128">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6">
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B129" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C129" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D129">
         <v>8345852</v>
@@ -3694,19 +3307,16 @@
       <c r="E129">
         <v>1</v>
       </c>
-      <c r="F129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6">
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B130" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C130" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D130">
         <v>59484639</v>
@@ -3714,19 +3324,16 @@
       <c r="E130">
         <v>1</v>
       </c>
-      <c r="F130">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6">
+    </row>
+    <row r="131" spans="1:5">
       <c r="A131" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C131" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D131">
         <v>29991441</v>
@@ -3734,19 +3341,16 @@
       <c r="E131">
         <v>1</v>
       </c>
-      <c r="F131">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6">
+    </row>
+    <row r="132" spans="1:5">
       <c r="A132" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B132" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C132" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D132">
         <v>8590995</v>
@@ -3754,19 +3358,16 @@
       <c r="E132">
         <v>1</v>
       </c>
-      <c r="F132">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6">
+    </row>
+    <row r="133" spans="1:5">
       <c r="A133" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B133" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C133" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D133">
         <v>3475185</v>
@@ -3774,19 +3375,16 @@
       <c r="E133">
         <v>1</v>
       </c>
-      <c r="F133">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6">
+    </row>
+    <row r="134" spans="1:5">
       <c r="A134" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B134" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C134" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D134">
         <v>8387808</v>
@@ -3794,19 +3392,16 @@
       <c r="E134">
         <v>1</v>
       </c>
-      <c r="F134">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6">
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C135" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D135">
         <v>121020072</v>
@@ -3814,19 +3409,16 @@
       <c r="E135">
         <v>1</v>
       </c>
-      <c r="F135">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6">
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C136" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D136">
         <v>76098531</v>
@@ -3834,19 +3426,16 @@
       <c r="E136">
         <v>1</v>
       </c>
-      <c r="F136">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6">
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C137" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D137">
         <v>74533750</v>
@@ -3854,19 +3443,16 @@
       <c r="E137">
         <v>1</v>
       </c>
-      <c r="F137">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6">
+    </row>
+    <row r="138" spans="1:5">
       <c r="A138" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C138" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D138">
         <v>97851198</v>
@@ -3874,19 +3460,16 @@
       <c r="E138">
         <v>1</v>
       </c>
-      <c r="F138">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6">
+    </row>
+    <row r="139" spans="1:5">
       <c r="A139" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C139" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D139">
         <v>58474121</v>
@@ -3894,19 +3477,16 @@
       <c r="E139">
         <v>2</v>
       </c>
-      <c r="F139">
-        <v>27.5</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6">
+    </row>
+    <row r="140" spans="1:5">
       <c r="A140" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C140" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D140">
         <v>9262953</v>
@@ -3914,19 +3494,16 @@
       <c r="E140">
         <v>2</v>
       </c>
-      <c r="F140">
-        <v>46.5</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6">
+    </row>
+    <row r="141" spans="1:5">
       <c r="A141" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C141" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D141">
         <v>24271952</v>
@@ -3934,19 +3511,16 @@
       <c r="E141">
         <v>2</v>
       </c>
-      <c r="F141">
-        <v>90.5</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6">
+    </row>
+    <row r="142" spans="1:5">
       <c r="A142" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C142" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D142">
         <v>25255876</v>
@@ -3954,19 +3528,16 @@
       <c r="E142">
         <v>2</v>
       </c>
-      <c r="F142">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6">
+    </row>
+    <row r="143" spans="1:5">
       <c r="A143" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C143" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D143">
         <v>59406989</v>
@@ -3974,27 +3545,21 @@
       <c r="E143">
         <v>1</v>
       </c>
-      <c r="F143">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6">
+    </row>
+    <row r="144" spans="1:5">
       <c r="A144" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C144" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D144">
         <v>29261051</v>
       </c>
       <c r="E144">
-        <v>1</v>
-      </c>
-      <c r="F144">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rewrote pages per session function and removed some redundant code.  The run time for the whole api log file was reduced from 1 hour to 4 minutes.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="248">
   <si>
     <t>company_name</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Sessions</t>
+  </si>
+  <si>
+    <t>Pages / Session</t>
   </si>
   <si>
     <t>Signature Consultants</t>
@@ -1112,13 +1115,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E144"/>
+  <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1134,16 +1137,19 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D2">
         <v>1874506</v>
@@ -1151,16 +1157,19 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D3">
         <v>88581275</v>
@@ -1168,16 +1177,19 @@
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D4">
         <v>2277</v>
@@ -1185,16 +1197,19 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D5">
         <v>94943308</v>
@@ -1202,16 +1217,19 @@
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D6">
         <v>9643371</v>
@@ -1219,16 +1237,19 @@
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D7">
         <v>3487433</v>
@@ -1236,16 +1257,19 @@
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D8">
         <v>29015547</v>
@@ -1253,16 +1277,19 @@
       <c r="E8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D9">
         <v>10710256</v>
@@ -1270,16 +1297,19 @@
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C10" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D10">
         <v>22837572</v>
@@ -1287,16 +1317,19 @@
       <c r="E10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D11">
         <v>120220674</v>
@@ -1304,16 +1337,19 @@
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D12">
         <v>87584491</v>
@@ -1321,16 +1357,19 @@
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C13" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D13">
         <v>62481418</v>
@@ -1338,16 +1377,19 @@
       <c r="E13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C14" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D14">
         <v>18304937</v>
@@ -1355,16 +1397,19 @@
       <c r="E14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C15" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D15">
         <v>76260666</v>
@@ -1372,16 +1417,19 @@
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C16" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D16">
         <v>122882133</v>
@@ -1389,16 +1437,19 @@
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C17" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D17">
         <v>427654</v>
@@ -1406,16 +1457,19 @@
       <c r="E17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D18">
         <v>1274211</v>
@@ -1423,16 +1477,19 @@
       <c r="E18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C19" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D19">
         <v>63243298</v>
@@ -1440,16 +1497,19 @@
       <c r="E19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C20" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D20">
         <v>107353422</v>
@@ -1457,16 +1517,19 @@
       <c r="E20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C21" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D21">
         <v>114279008</v>
@@ -1474,16 +1537,19 @@
       <c r="E21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C22" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D22">
         <v>62276135</v>
@@ -1491,16 +1557,19 @@
       <c r="E22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C23" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D23">
         <v>61131136</v>
@@ -1508,16 +1577,19 @@
       <c r="E23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C24" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D24">
         <v>8334706</v>
@@ -1525,16 +1597,19 @@
       <c r="E24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C25" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D25">
         <v>120294900</v>
@@ -1542,13 +1617,16 @@
       <c r="E25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D26">
         <v>123181958</v>
@@ -1556,16 +1634,19 @@
       <c r="E26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D27">
         <v>59014</v>
@@ -1573,16 +1654,19 @@
       <c r="E27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C28" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D28">
         <v>118357638</v>
@@ -1590,16 +1674,19 @@
       <c r="E28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C29" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D29">
         <v>50919072</v>
@@ -1607,16 +1694,19 @@
       <c r="E29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C30" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D30">
         <v>206865</v>
@@ -1624,16 +1714,19 @@
       <c r="E30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C31" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D31">
         <v>55091</v>
@@ -1641,16 +1734,19 @@
       <c r="E31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C32" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D32">
         <v>23077089</v>
@@ -1658,16 +1754,19 @@
       <c r="E32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C33" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D33">
         <v>324782</v>
@@ -1675,16 +1774,19 @@
       <c r="E33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C34" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D34">
         <v>50792754</v>
@@ -1692,16 +1794,19 @@
       <c r="E34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C35" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D35">
         <v>1657209</v>
@@ -1709,16 +1814,19 @@
       <c r="E35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C36" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D36">
         <v>29363767</v>
@@ -1726,16 +1834,19 @@
       <c r="E36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C37" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D37">
         <v>119753147</v>
@@ -1743,16 +1854,19 @@
       <c r="E37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C38" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D38">
         <v>8813570</v>
@@ -1760,16 +1874,19 @@
       <c r="E38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C39" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D39">
         <v>9716409</v>
@@ -1777,16 +1894,19 @@
       <c r="E39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C40" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D40">
         <v>3439734</v>
@@ -1794,16 +1914,19 @@
       <c r="E40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C41" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D41">
         <v>28166261</v>
@@ -1811,16 +1934,19 @@
       <c r="E41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C42" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D42">
         <v>110164086</v>
@@ -1828,16 +1954,19 @@
       <c r="E42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C43" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D43">
         <v>65549391</v>
@@ -1845,16 +1974,19 @@
       <c r="E43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C44" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D44">
         <v>152167</v>
@@ -1862,16 +1994,19 @@
       <c r="E44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C45" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D45">
         <v>3546637</v>
@@ -1879,16 +2014,19 @@
       <c r="E45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C46" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D46">
         <v>672468</v>
@@ -1896,16 +2034,19 @@
       <c r="E46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C47" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D47">
         <v>88581346</v>
@@ -1913,16 +2054,19 @@
       <c r="E47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C48" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D48">
         <v>333292</v>
@@ -1930,16 +2074,19 @@
       <c r="E48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C49" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D49">
         <v>120353825</v>
@@ -1947,16 +2094,19 @@
       <c r="E49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C50" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D50">
         <v>114803999</v>
@@ -1964,16 +2114,19 @@
       <c r="E50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C51" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D51">
         <v>121066621</v>
@@ -1981,16 +2134,19 @@
       <c r="E51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C52" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D52">
         <v>114363338</v>
@@ -1998,16 +2154,19 @@
       <c r="E52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C53" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D53">
         <v>8870506</v>
@@ -2015,16 +2174,19 @@
       <c r="E53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C54" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D54">
         <v>9636101</v>
@@ -2032,16 +2194,19 @@
       <c r="E54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C55" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D55">
         <v>24505728</v>
@@ -2049,16 +2214,19 @@
       <c r="E55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C56" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D56">
         <v>114413047</v>
@@ -2066,16 +2234,19 @@
       <c r="E56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C57" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D57">
         <v>3383279</v>
@@ -2083,16 +2254,19 @@
       <c r="E57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C58" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D58">
         <v>18261037</v>
@@ -2100,16 +2274,19 @@
       <c r="E58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B59" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C59" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D59">
         <v>50792693</v>
@@ -2117,16 +2294,19 @@
       <c r="E59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C60" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D60">
         <v>65419794</v>
@@ -2134,16 +2314,19 @@
       <c r="E60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C61" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D61">
         <v>111937346</v>
@@ -2151,16 +2334,19 @@
       <c r="E61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C62" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D62">
         <v>25049946</v>
@@ -2168,16 +2354,19 @@
       <c r="E62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C63" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D63">
         <v>62142906</v>
@@ -2185,16 +2374,19 @@
       <c r="E63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C64" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D64">
         <v>411470</v>
@@ -2202,16 +2394,19 @@
       <c r="E64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C65" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D65">
         <v>77504470</v>
@@ -2219,16 +2414,19 @@
       <c r="E65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C66" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D66">
         <v>110129535</v>
@@ -2236,16 +2434,19 @@
       <c r="E66">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="F66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C67" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D67">
         <v>61358666</v>
@@ -2253,16 +2454,19 @@
       <c r="E67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C68" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D68">
         <v>116578742</v>
@@ -2270,16 +2474,19 @@
       <c r="E68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="F68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B69" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C69" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D69">
         <v>62085175</v>
@@ -2287,16 +2494,19 @@
       <c r="E69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="F69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B70" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C70" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D70">
         <v>75933854</v>
@@ -2304,16 +2514,19 @@
       <c r="E70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="F70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C71" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D71">
         <v>75925683</v>
@@ -2321,16 +2534,19 @@
       <c r="E71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="F71">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B72" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C72" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D72">
         <v>62192622</v>
@@ -2338,16 +2554,19 @@
       <c r="E72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="F72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C73" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D73">
         <v>3474028</v>
@@ -2355,16 +2574,19 @@
       <c r="E73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="F73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B74" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C74" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D74">
         <v>2120924</v>
@@ -2372,16 +2594,19 @@
       <c r="E74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="F74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B75" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C75" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D75">
         <v>574762</v>
@@ -2389,16 +2614,19 @@
       <c r="E75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="F75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B76" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C76" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D76">
         <v>119309550</v>
@@ -2406,16 +2634,19 @@
       <c r="E76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="F76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B77" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C77" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D77">
         <v>79984352</v>
@@ -2423,16 +2654,19 @@
       <c r="E77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="F77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C78" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D78">
         <v>96316606</v>
@@ -2440,16 +2674,19 @@
       <c r="E78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="F78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C79" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D79">
         <v>121239002</v>
@@ -2457,16 +2694,19 @@
       <c r="E79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="F79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C80" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D80">
         <v>65690454</v>
@@ -2474,16 +2714,19 @@
       <c r="E80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="F80">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B81" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C81" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D81">
         <v>48861</v>
@@ -2491,16 +2734,19 @@
       <c r="E81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="F81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B82" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C82" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D82">
         <v>441104</v>
@@ -2508,16 +2754,19 @@
       <c r="E82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="F82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C83" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D83">
         <v>417598</v>
@@ -2525,16 +2774,19 @@
       <c r="E83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="F83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B84" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C84" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D84">
         <v>282236</v>
@@ -2542,16 +2794,19 @@
       <c r="E84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="F84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B85" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C85" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D85">
         <v>3617</v>
@@ -2559,16 +2814,19 @@
       <c r="E85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="F85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C86" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D86">
         <v>64789992</v>
@@ -2576,16 +2834,19 @@
       <c r="E86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="F86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C87" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D87">
         <v>53478381</v>
@@ -2593,16 +2854,19 @@
       <c r="E87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="F87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C88" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D88">
         <v>74750637</v>
@@ -2610,16 +2874,19 @@
       <c r="E88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="F88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C89" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D89">
         <v>24551256</v>
@@ -2627,16 +2894,19 @@
       <c r="E89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="F89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C90" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D90">
         <v>27515672</v>
@@ -2644,16 +2914,19 @@
       <c r="E90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="F90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C91" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D91">
         <v>285202</v>
@@ -2661,16 +2934,19 @@
       <c r="E91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="F91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C92" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D92">
         <v>330734</v>
@@ -2678,16 +2954,19 @@
       <c r="E92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="F92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C93" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D93">
         <v>66899178</v>
@@ -2695,16 +2974,19 @@
       <c r="E93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="F93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C94" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D94">
         <v>23781648</v>
@@ -2712,16 +2994,19 @@
       <c r="E94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="F94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C95" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D95">
         <v>89580408</v>
@@ -2729,16 +3014,19 @@
       <c r="E95">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="F95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C96" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D96">
         <v>59702148</v>
@@ -2746,16 +3034,19 @@
       <c r="E96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="F96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B97" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C97" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D97">
         <v>29344533</v>
@@ -2763,16 +3054,19 @@
       <c r="E97">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="F97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C98" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D98">
         <v>3652496</v>
@@ -2780,16 +3074,19 @@
       <c r="E98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="F98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C99" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D99">
         <v>115048979</v>
@@ -2797,16 +3094,19 @@
       <c r="E99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="F99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C100" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D100">
         <v>122253967</v>
@@ -2814,16 +3114,19 @@
       <c r="E100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:5">
+      <c r="F100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C101" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D101">
         <v>76317857</v>
@@ -2831,16 +3134,19 @@
       <c r="E101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="F101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C102" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D102">
         <v>28916725</v>
@@ -2848,16 +3154,19 @@
       <c r="E102">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="F102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C103" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D103">
         <v>116500972</v>
@@ -2865,16 +3174,19 @@
       <c r="E103">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="F103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C104" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D104">
         <v>121155406</v>
@@ -2882,16 +3194,19 @@
       <c r="E104">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="F104">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C105" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D105">
         <v>113083468</v>
@@ -2899,16 +3214,19 @@
       <c r="E105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="F105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C106" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D106">
         <v>121500828</v>
@@ -2916,16 +3234,19 @@
       <c r="E106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="F106">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C107" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D107">
         <v>61673614</v>
@@ -2933,16 +3254,19 @@
       <c r="E107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="F107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C108" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D108">
         <v>107353754</v>
@@ -2950,16 +3274,19 @@
       <c r="E108">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="F108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C109" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D109">
         <v>94430121</v>
@@ -2967,16 +3294,19 @@
       <c r="E109">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="F109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C110" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D110">
         <v>30166573</v>
@@ -2984,16 +3314,19 @@
       <c r="E110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="F110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C111" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D111">
         <v>1874075</v>
@@ -3001,16 +3334,19 @@
       <c r="E111">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:5">
+      <c r="F111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C112" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D112">
         <v>63056166</v>
@@ -3018,16 +3354,19 @@
       <c r="E112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:5">
+      <c r="F112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C113" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D113">
         <v>73509114</v>
@@ -3035,16 +3374,19 @@
       <c r="E113">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:5">
+      <c r="F113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C114" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D114">
         <v>4009456</v>
@@ -3052,16 +3394,19 @@
       <c r="E114">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:5">
+      <c r="F114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C115" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D115">
         <v>63237387</v>
@@ -3069,16 +3414,19 @@
       <c r="E115">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:5">
+      <c r="F115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C116" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D116">
         <v>61659652</v>
@@ -3086,16 +3434,19 @@
       <c r="E116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:5">
+      <c r="F116">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C117" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D117">
         <v>121092023</v>
@@ -3103,16 +3454,19 @@
       <c r="E117">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:5">
+      <c r="F117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C118" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D118">
         <v>10615945</v>
@@ -3120,16 +3474,19 @@
       <c r="E118">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:5">
+      <c r="F118">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C119" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D119">
         <v>60358057</v>
@@ -3137,16 +3494,19 @@
       <c r="E119">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:5">
+      <c r="F119">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C120" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D120">
         <v>114799829</v>
@@ -3154,16 +3514,19 @@
       <c r="E120">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:5">
+      <c r="F120">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C121" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D121">
         <v>3840295</v>
@@ -3171,16 +3534,19 @@
       <c r="E121">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:5">
+      <c r="F121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C122" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D122">
         <v>29684833</v>
@@ -3188,16 +3554,19 @@
       <c r="E122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:5">
+      <c r="F122">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C123" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D123">
         <v>22983616</v>
@@ -3205,16 +3574,19 @@
       <c r="E123">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:5">
+      <c r="F123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C124" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D124">
         <v>10020982</v>
@@ -3222,16 +3594,19 @@
       <c r="E124">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:5">
+      <c r="F124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C125" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D125">
         <v>121070994</v>
@@ -3239,16 +3614,19 @@
       <c r="E125">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:5">
+      <c r="F125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C126" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D126">
         <v>1047511</v>
@@ -3256,16 +3634,19 @@
       <c r="E126">
         <v>2</v>
       </c>
-    </row>
-    <row r="127" spans="1:5">
+      <c r="F126">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C127" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D127">
         <v>78172883</v>
@@ -3273,16 +3654,19 @@
       <c r="E127">
         <v>2</v>
       </c>
-    </row>
-    <row r="128" spans="1:5">
+      <c r="F127">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C128" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D128">
         <v>37515</v>
@@ -3290,16 +3674,19 @@
       <c r="E128">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:5">
+      <c r="F128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C129" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D129">
         <v>8345852</v>
@@ -3307,16 +3694,19 @@
       <c r="E129">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:5">
+      <c r="F129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B130" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C130" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D130">
         <v>59484639</v>
@@ -3324,16 +3714,19 @@
       <c r="E130">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:5">
+      <c r="F130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
       <c r="A131" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B131" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C131" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D131">
         <v>29991441</v>
@@ -3341,16 +3734,19 @@
       <c r="E131">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:5">
+      <c r="F131">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
       <c r="A132" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B132" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C132" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D132">
         <v>8590995</v>
@@ -3358,16 +3754,19 @@
       <c r="E132">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:5">
+      <c r="F132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B133" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C133" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D133">
         <v>3475185</v>
@@ -3375,16 +3774,19 @@
       <c r="E133">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="F133">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B134" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C134" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D134">
         <v>8387808</v>
@@ -3392,16 +3794,19 @@
       <c r="E134">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:5">
+      <c r="F134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B135" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C135" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D135">
         <v>121020072</v>
@@ -3409,16 +3814,19 @@
       <c r="E135">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:5">
+      <c r="F135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
       <c r="A136" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B136" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C136" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D136">
         <v>76098531</v>
@@ -3426,16 +3834,19 @@
       <c r="E136">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:5">
+      <c r="F136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
       <c r="A137" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B137" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C137" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D137">
         <v>74533750</v>
@@ -3443,16 +3854,19 @@
       <c r="E137">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:5">
+      <c r="F137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B138" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C138" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D138">
         <v>97851198</v>
@@ -3460,16 +3874,19 @@
       <c r="E138">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:5">
+      <c r="F138">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B139" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C139" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D139">
         <v>58474121</v>
@@ -3477,16 +3894,19 @@
       <c r="E139">
         <v>2</v>
       </c>
-    </row>
-    <row r="140" spans="1:5">
+      <c r="F139">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B140" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C140" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D140">
         <v>9262953</v>
@@ -3494,16 +3914,19 @@
       <c r="E140">
         <v>2</v>
       </c>
-    </row>
-    <row r="141" spans="1:5">
+      <c r="F140">
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
       <c r="A141" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B141" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C141" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D141">
         <v>24271952</v>
@@ -3511,16 +3934,19 @@
       <c r="E141">
         <v>2</v>
       </c>
-    </row>
-    <row r="142" spans="1:5">
+      <c r="F141">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B142" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C142" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D142">
         <v>25255876</v>
@@ -3528,16 +3954,19 @@
       <c r="E142">
         <v>2</v>
       </c>
-    </row>
-    <row r="143" spans="1:5">
+      <c r="F142">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
       <c r="A143" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B143" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C143" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D143">
         <v>59406989</v>
@@ -3545,21 +3974,27 @@
       <c r="E143">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:5">
+      <c r="F143">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B144" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C144" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D144">
         <v>29261051</v>
       </c>
       <c r="E144">
+        <v>1</v>
+      </c>
+      <c r="F144">
         <v>1</v>
       </c>
     </row>

</xml_diff>